<commit_message>
Updated clean data and readme
</commit_message>
<xml_diff>
--- a/data/Raw_Study_Responses.xlsx
+++ b/data/Raw_Study_Responses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neiljones/Documents/Files/CodingProjects/Python/Projects/CollegeMajorvsCovid-Revisited/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280E5EF5-4B06-0F48-A961-8F6956945447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568DA813-2592-354B-9C03-5A6B11A06F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="18200" windowHeight="8500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="24780" windowHeight="14560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="74">
   <si>
     <t>Timestamp</t>
   </si>
@@ -208,12 +208,6 @@
     <t>Secondary Education</t>
   </si>
   <si>
-    <t>Managment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Undecided </t>
-  </si>
-  <si>
     <t>Chemistry</t>
   </si>
   <si>
@@ -235,9 +229,6 @@
     <t>Substance Abuse Counseling</t>
   </si>
   <si>
-    <t>Master in Admin</t>
-  </si>
-  <si>
     <t xml:space="preserve">Biology </t>
   </si>
   <si>
@@ -245,6 +236,12 @@
   </si>
   <si>
     <t>My college classes have updated their curriculum in response to Covid-19</t>
+  </si>
+  <si>
+    <t>Master in Administration</t>
+  </si>
+  <si>
+    <t>Management</t>
   </si>
 </sst>
 </file>
@@ -615,9 +612,9 @@
   </sheetPr>
   <dimension ref="A1:P107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -673,7 +670,7 @@
         <v>14</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2939,6 +2936,7 @@
       <c r="D47" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="E47" s="2"/>
       <c r="F47" s="2" t="s">
         <v>32</v>
       </c>
@@ -3584,7 +3582,7 @@
         <v>39</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>47</v>
@@ -3634,7 +3632,7 @@
         <v>26</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>18</v>
@@ -3984,7 +3982,7 @@
         <v>26</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>37</v>
@@ -4034,7 +4032,7 @@
         <v>16</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>47</v>
@@ -4184,7 +4182,7 @@
         <v>16</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>47</v>
@@ -4284,7 +4282,7 @@
         <v>26</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>47</v>
@@ -4334,7 +4332,7 @@
         <v>26</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>37</v>
@@ -4384,7 +4382,7 @@
         <v>16</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>37</v>
@@ -4434,7 +4432,7 @@
         <v>26</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>37</v>
@@ -4634,7 +4632,7 @@
         <v>16</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>37</v>
@@ -4834,7 +4832,7 @@
         <v>26</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>32</v>
@@ -4934,7 +4932,7 @@
         <v>26</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>18</v>
@@ -4984,7 +4982,7 @@
         <v>26</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>35</v>
@@ -5034,7 +5032,7 @@
         <v>16</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>32</v>
@@ -5084,7 +5082,7 @@
         <v>16</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>35</v>
@@ -5884,7 +5882,7 @@
         <v>26</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>35</v>

</xml_diff>